<commit_message>
Added Error Handler module to project
</commit_message>
<xml_diff>
--- a/sample excel upload file.xlsx
+++ b/sample excel upload file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a15fa1d46e479/Pictures/Programming/edureka/other projects/famersdb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{4A949238-DD98-494A-B49C-B0E9EFC9F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{242A4827-FD58-4286-A6C1-53460452C0FB}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{4A949238-DD98-494A-B49C-B0E9EFC9F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31E2FFB1-62A7-4B9F-A1BA-03D008D66342}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B7C111A7-4628-4EF4-B6B9-D9575148AAE1}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added loanAmount to farmer
</commit_message>
<xml_diff>
--- a/sample excel upload file.xlsx
+++ b/sample excel upload file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a04a15fa1d46e479/Pictures/Programming/edureka/other projects/famersdb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{4A949238-DD98-494A-B49C-B0E9EFC9F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31E2FFB1-62A7-4B9F-A1BA-03D008D66342}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{4A949238-DD98-494A-B49C-B0E9EFC9F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2205BC37-A280-40CB-9517-9D7B2886224C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B7C111A7-4628-4EF4-B6B9-D9575148AAE1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="48">
   <si>
     <t>company</t>
   </si>
@@ -156,25 +156,31 @@
     <t>"2002-05-05"</t>
   </si>
   <si>
-    <t>600001/66/2</t>
-  </si>
-  <si>
-    <t>600001/66/3</t>
-  </si>
-  <si>
-    <t>600001/66/4</t>
-  </si>
-  <si>
-    <t>600001/66/5</t>
-  </si>
-  <si>
-    <t>600001/66/6</t>
-  </si>
-  <si>
-    <t>600001/66/7</t>
-  </si>
-  <si>
-    <t>600001/66/8</t>
+    <t>loanAmount</t>
+  </si>
+  <si>
+    <t>600001/22/1</t>
+  </si>
+  <si>
+    <t>600001/22/2</t>
+  </si>
+  <si>
+    <t>600001/22/3</t>
+  </si>
+  <si>
+    <t>600001/22/4</t>
+  </si>
+  <si>
+    <t>600001/22/5</t>
+  </si>
+  <si>
+    <t>600001/22/6</t>
+  </si>
+  <si>
+    <t>600001/22/7</t>
+  </si>
+  <si>
+    <t>600001/22/8</t>
   </si>
 </sst>
 </file>
@@ -222,11 +228,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DF3571-C207-455B-8530-4ACC29089DC8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +569,7 @@
     <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -580,8 +588,11 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -589,7 +600,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>38</v>
@@ -600,8 +611,11 @@
       <c r="F2">
         <v>2024</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="5">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -609,7 +623,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>38</v>
@@ -620,8 +634,11 @@
       <c r="F3">
         <v>2024</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -629,7 +646,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>38</v>
@@ -640,8 +657,11 @@
       <c r="F4">
         <v>2024</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="4">
+        <v>51003.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -649,7 +669,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>38</v>
@@ -660,8 +680,11 @@
       <c r="F5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -669,7 +692,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>38</v>
@@ -680,8 +703,11 @@
       <c r="F6">
         <v>2024</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -689,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>38</v>
@@ -700,8 +726,11 @@
       <c r="F7">
         <v>2024</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -709,7 +738,7 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>38</v>
@@ -720,8 +749,11 @@
       <c r="F8">
         <v>2024</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -729,7 +761,7 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>38</v>
@@ -739,6 +771,9 @@
       </c>
       <c r="F9">
         <v>2024</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>